<commit_message>
Amended WP1 data dictionaires
1) child_ids have been changed to "text" data type
2) labels amended in the yearly-repeated data dictionary
3) categories corrected in the yearly and non-repeated data dictionaries
4) cat and dog variables added to the yearly and non-repeated data dictionaries
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_monthly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_monthly_repeated.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10909"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/1_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ProjectGroups\LifeCycle\Data dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3658223B-DE1F-2A46-9B58-D84AF4785288}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>name</t>
   </si>
@@ -105,12 +104,15 @@
   </si>
   <si>
     <t>Unique identifier for the row in Opal</t>
+  </si>
+  <si>
+    <t>text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,8 +187,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -644,23 +646,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="42.5" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="15.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -729,7 +731,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -798,22 +800,20 @@
       <c r="BF2"/>
       <c r="BG2"/>
     </row>
-    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="B3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E3"/>
     </row>
-    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -828,7 +828,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -842,7 +842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -857,7 +857,7 @@
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -871,7 +871,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -885,7 +885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -909,20 +909,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="12.85546875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>